<commit_message>
Added matches from May 4th, 2023.
</commit_message>
<xml_diff>
--- a/exports/elo_time_table.xlsx
+++ b/exports/elo_time_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD98"/>
+  <dimension ref="A1:AD103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4390,6 +4390,216 @@
       <c r="AC98" t="inlineStr"/>
       <c r="AD98" t="inlineStr"/>
     </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="n">
+        <v>1440.937491956877</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1320.599411601501</v>
+      </c>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr"/>
+      <c r="S99" t="n">
+        <v>1300.147034719307</v>
+      </c>
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr"/>
+      <c r="Y99" t="inlineStr"/>
+      <c r="Z99" t="inlineStr"/>
+      <c r="AA99" t="inlineStr"/>
+      <c r="AB99" t="inlineStr"/>
+      <c r="AC99" t="inlineStr"/>
+      <c r="AD99" t="n">
+        <v>1058.266119428515</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="n">
+        <v>1455.524158726644</v>
+      </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="n">
+        <v>1188.642712845706</v>
+      </c>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
+      <c r="R100" t="inlineStr"/>
+      <c r="S100" t="n">
+        <v>1314.733701489074</v>
+      </c>
+      <c r="T100" t="inlineStr"/>
+      <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr"/>
+      <c r="Y100" t="inlineStr"/>
+      <c r="Z100" t="inlineStr"/>
+      <c r="AA100" t="n">
+        <v>1219.740685506919</v>
+      </c>
+      <c r="AB100" t="inlineStr"/>
+      <c r="AC100" t="inlineStr"/>
+      <c r="AD100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="n">
+        <v>1475.175154270586</v>
+      </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="n">
+        <v>1210.880075869332</v>
+      </c>
+      <c r="I101" t="n">
+        <v>986.6306877551247</v>
+      </c>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
+      <c r="R101" t="inlineStr"/>
+      <c r="S101" t="n">
+        <v>1334.384697033016</v>
+      </c>
+      <c r="T101" t="inlineStr"/>
+      <c r="U101" t="inlineStr"/>
+      <c r="V101" t="inlineStr"/>
+      <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr"/>
+      <c r="Y101" t="inlineStr"/>
+      <c r="Z101" t="inlineStr"/>
+      <c r="AA101" t="inlineStr"/>
+      <c r="AB101" t="inlineStr"/>
+      <c r="AC101" t="inlineStr"/>
+      <c r="AD101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="n">
+        <v>1487.171735435872</v>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="n">
+        <v>1198.883494704046</v>
+      </c>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr"/>
+      <c r="R102" t="inlineStr"/>
+      <c r="S102" t="n">
+        <v>1346.381278198303</v>
+      </c>
+      <c r="T102" t="n">
+        <v>1198.228992509007</v>
+      </c>
+      <c r="U102" t="inlineStr"/>
+      <c r="V102" t="inlineStr"/>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr"/>
+      <c r="Y102" t="inlineStr"/>
+      <c r="Z102" t="inlineStr"/>
+      <c r="AA102" t="inlineStr"/>
+      <c r="AB102" t="inlineStr"/>
+      <c r="AC102" t="inlineStr"/>
+      <c r="AD102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="n">
+        <v>1537.121990870036</v>
+      </c>
+      <c r="G103" t="n">
+        <v>1270.649156167338</v>
+      </c>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="n">
+        <v>1138.692457411543</v>
+      </c>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
+      <c r="R103" t="inlineStr"/>
+      <c r="S103" t="n">
+        <v>1396.331533632466</v>
+      </c>
+      <c r="T103" t="inlineStr"/>
+      <c r="U103" t="inlineStr"/>
+      <c r="V103" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr"/>
+      <c r="Y103" t="inlineStr"/>
+      <c r="Z103" t="inlineStr"/>
+      <c r="AA103" t="inlineStr"/>
+      <c r="AB103" t="inlineStr"/>
+      <c r="AC103" t="inlineStr"/>
+      <c r="AD103" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added beach week and "the last roll" games.
</commit_message>
<xml_diff>
--- a/exports/elo_time_table.xlsx
+++ b/exports/elo_time_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD103"/>
+  <dimension ref="A1:AH115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Levin Lee</t>
+          <t>Kevin Lee</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
@@ -577,6 +577,26 @@
       <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Cassie Deering</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Spencer Harris</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Bronte Sundstrom</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Parker Simpson</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Abby LeahFriend</t>
         </is>
       </c>
     </row>
@@ -621,6 +641,10 @@
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -663,6 +687,10 @@
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -705,6 +733,10 @@
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -747,6 +779,10 @@
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
       <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -789,6 +825,10 @@
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
       <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -831,6 +871,10 @@
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -873,6 +917,10 @@
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -915,6 +963,10 @@
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
       <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -957,6 +1009,10 @@
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -999,6 +1055,10 @@
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1041,6 +1101,10 @@
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
       <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1083,6 +1147,10 @@
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1125,6 +1193,10 @@
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1167,6 +1239,10 @@
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1205,6 +1281,10 @@
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1243,6 +1323,10 @@
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1281,6 +1365,10 @@
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="inlineStr"/>
       <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1319,6 +1407,10 @@
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="inlineStr"/>
       <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1357,6 +1449,10 @@
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="inlineStr"/>
       <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1395,6 +1491,10 @@
       <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1433,6 +1533,10 @@
       <c r="AB22" t="inlineStr"/>
       <c r="AC22" t="inlineStr"/>
       <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1471,6 +1575,10 @@
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="inlineStr"/>
       <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1509,6 +1617,10 @@
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1547,6 +1659,10 @@
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1585,6 +1701,10 @@
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1623,6 +1743,10 @@
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1661,6 +1785,10 @@
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
       <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1699,6 +1827,10 @@
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="inlineStr"/>
       <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1737,6 +1869,10 @@
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="inlineStr"/>
       <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1775,6 +1911,10 @@
       <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1813,6 +1953,10 @@
       <c r="AB32" t="inlineStr"/>
       <c r="AC32" t="inlineStr"/>
       <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1851,6 +1995,10 @@
       <c r="AB33" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1889,6 +2037,10 @@
       <c r="AB34" t="inlineStr"/>
       <c r="AC34" t="inlineStr"/>
       <c r="AD34" t="inlineStr"/>
+      <c r="AE34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr"/>
+      <c r="AG34" t="inlineStr"/>
+      <c r="AH34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1927,6 +2079,10 @@
       <c r="AB35" t="inlineStr"/>
       <c r="AC35" t="inlineStr"/>
       <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr"/>
+      <c r="AG35" t="inlineStr"/>
+      <c r="AH35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1965,6 +2121,10 @@
       <c r="AB36" t="inlineStr"/>
       <c r="AC36" t="inlineStr"/>
       <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr"/>
+      <c r="AG36" t="inlineStr"/>
+      <c r="AH36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2003,6 +2163,10 @@
       <c r="AB37" t="inlineStr"/>
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
+      <c r="AE37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="inlineStr"/>
+      <c r="AH37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2041,6 +2205,10 @@
       <c r="AB38" t="inlineStr"/>
       <c r="AC38" t="inlineStr"/>
       <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr"/>
+      <c r="AG38" t="inlineStr"/>
+      <c r="AH38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2079,6 +2247,10 @@
       <c r="AB39" t="inlineStr"/>
       <c r="AC39" t="inlineStr"/>
       <c r="AD39" t="inlineStr"/>
+      <c r="AE39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="inlineStr"/>
+      <c r="AH39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2117,6 +2289,10 @@
       <c r="AB40" t="inlineStr"/>
       <c r="AC40" t="inlineStr"/>
       <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2155,6 +2331,10 @@
       <c r="AB41" t="inlineStr"/>
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr"/>
+      <c r="AE41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr"/>
+      <c r="AH41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2193,6 +2373,10 @@
       <c r="AB42" t="inlineStr"/>
       <c r="AC42" t="inlineStr"/>
       <c r="AD42" t="inlineStr"/>
+      <c r="AE42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="inlineStr"/>
+      <c r="AH42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2231,6 +2415,10 @@
       <c r="AB43" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
+      <c r="AH43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2269,6 +2457,10 @@
       <c r="AB44" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
       <c r="AD44" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
+      <c r="AH44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2311,6 +2503,10 @@
       <c r="AB45" t="inlineStr"/>
       <c r="AC45" t="inlineStr"/>
       <c r="AD45" t="inlineStr"/>
+      <c r="AE45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="inlineStr"/>
+      <c r="AH45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2353,6 +2549,10 @@
       <c r="AB46" t="inlineStr"/>
       <c r="AC46" t="inlineStr"/>
       <c r="AD46" t="inlineStr"/>
+      <c r="AE46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="inlineStr"/>
+      <c r="AH46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2395,6 +2595,10 @@
       <c r="AB47" t="inlineStr"/>
       <c r="AC47" t="inlineStr"/>
       <c r="AD47" t="inlineStr"/>
+      <c r="AE47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="inlineStr"/>
+      <c r="AH47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2437,6 +2641,10 @@
       <c r="AB48" t="inlineStr"/>
       <c r="AC48" t="inlineStr"/>
       <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2479,6 +2687,10 @@
       <c r="AB49" t="inlineStr"/>
       <c r="AC49" t="inlineStr"/>
       <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2521,6 +2733,10 @@
       <c r="AB50" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
       <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2563,6 +2779,10 @@
       <c r="AB51" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
       <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2605,6 +2825,10 @@
       <c r="AB52" t="inlineStr"/>
       <c r="AC52" t="inlineStr"/>
       <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2647,6 +2871,10 @@
       <c r="AB53" t="inlineStr"/>
       <c r="AC53" t="inlineStr"/>
       <c r="AD53" t="inlineStr"/>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr"/>
+      <c r="AH53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2689,6 +2917,10 @@
       <c r="AB54" t="inlineStr"/>
       <c r="AC54" t="inlineStr"/>
       <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2731,6 +2963,10 @@
       <c r="AB55" t="inlineStr"/>
       <c r="AC55" t="inlineStr"/>
       <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2773,6 +3009,10 @@
       <c r="AB56" t="inlineStr"/>
       <c r="AC56" t="inlineStr"/>
       <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2815,6 +3055,10 @@
       <c r="AB57" t="inlineStr"/>
       <c r="AC57" t="inlineStr"/>
       <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2857,6 +3101,10 @@
       <c r="AB58" t="inlineStr"/>
       <c r="AC58" t="inlineStr"/>
       <c r="AD58" t="inlineStr"/>
+      <c r="AE58" t="inlineStr"/>
+      <c r="AF58" t="inlineStr"/>
+      <c r="AG58" t="inlineStr"/>
+      <c r="AH58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2899,6 +3147,10 @@
       <c r="AB59" t="inlineStr"/>
       <c r="AC59" t="inlineStr"/>
       <c r="AD59" t="inlineStr"/>
+      <c r="AE59" t="inlineStr"/>
+      <c r="AF59" t="inlineStr"/>
+      <c r="AG59" t="inlineStr"/>
+      <c r="AH59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2941,6 +3193,10 @@
       <c r="AB60" t="inlineStr"/>
       <c r="AC60" t="inlineStr"/>
       <c r="AD60" t="inlineStr"/>
+      <c r="AE60" t="inlineStr"/>
+      <c r="AF60" t="inlineStr"/>
+      <c r="AG60" t="inlineStr"/>
+      <c r="AH60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2983,6 +3239,10 @@
       <c r="AB61" t="inlineStr"/>
       <c r="AC61" t="inlineStr"/>
       <c r="AD61" t="inlineStr"/>
+      <c r="AE61" t="inlineStr"/>
+      <c r="AF61" t="inlineStr"/>
+      <c r="AG61" t="inlineStr"/>
+      <c r="AH61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3021,6 +3281,10 @@
       <c r="AB62" t="inlineStr"/>
       <c r="AC62" t="inlineStr"/>
       <c r="AD62" t="inlineStr"/>
+      <c r="AE62" t="inlineStr"/>
+      <c r="AF62" t="inlineStr"/>
+      <c r="AG62" t="inlineStr"/>
+      <c r="AH62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3059,6 +3323,10 @@
       <c r="AD63" t="n">
         <v>1186.140249136186</v>
       </c>
+      <c r="AE63" t="inlineStr"/>
+      <c r="AF63" t="inlineStr"/>
+      <c r="AG63" t="inlineStr"/>
+      <c r="AH63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3097,6 +3365,10 @@
         <v>1201.699690056111</v>
       </c>
       <c r="AD64" t="inlineStr"/>
+      <c r="AE64" t="inlineStr"/>
+      <c r="AF64" t="inlineStr"/>
+      <c r="AG64" t="inlineStr"/>
+      <c r="AH64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3135,6 +3407,10 @@
       <c r="AB65" t="inlineStr"/>
       <c r="AC65" t="inlineStr"/>
       <c r="AD65" t="inlineStr"/>
+      <c r="AE65" t="inlineStr"/>
+      <c r="AF65" t="inlineStr"/>
+      <c r="AG65" t="inlineStr"/>
+      <c r="AH65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3173,6 +3449,10 @@
       </c>
       <c r="AC66" t="inlineStr"/>
       <c r="AD66" t="inlineStr"/>
+      <c r="AE66" t="inlineStr"/>
+      <c r="AF66" t="inlineStr"/>
+      <c r="AG66" t="inlineStr"/>
+      <c r="AH66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -3211,6 +3491,10 @@
       <c r="AB67" t="inlineStr"/>
       <c r="AC67" t="inlineStr"/>
       <c r="AD67" t="inlineStr"/>
+      <c r="AE67" t="inlineStr"/>
+      <c r="AF67" t="inlineStr"/>
+      <c r="AG67" t="inlineStr"/>
+      <c r="AH67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3249,6 +3533,10 @@
       <c r="AB68" t="inlineStr"/>
       <c r="AC68" t="inlineStr"/>
       <c r="AD68" t="inlineStr"/>
+      <c r="AE68" t="inlineStr"/>
+      <c r="AF68" t="inlineStr"/>
+      <c r="AG68" t="inlineStr"/>
+      <c r="AH68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3287,6 +3575,10 @@
       <c r="AB69" t="inlineStr"/>
       <c r="AC69" t="inlineStr"/>
       <c r="AD69" t="inlineStr"/>
+      <c r="AE69" t="inlineStr"/>
+      <c r="AF69" t="inlineStr"/>
+      <c r="AG69" t="inlineStr"/>
+      <c r="AH69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3325,6 +3617,10 @@
       <c r="AB70" t="inlineStr"/>
       <c r="AC70" t="inlineStr"/>
       <c r="AD70" t="inlineStr"/>
+      <c r="AE70" t="inlineStr"/>
+      <c r="AF70" t="inlineStr"/>
+      <c r="AG70" t="inlineStr"/>
+      <c r="AH70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -3363,6 +3659,10 @@
       <c r="AB71" t="inlineStr"/>
       <c r="AC71" t="inlineStr"/>
       <c r="AD71" t="inlineStr"/>
+      <c r="AE71" t="inlineStr"/>
+      <c r="AF71" t="inlineStr"/>
+      <c r="AG71" t="inlineStr"/>
+      <c r="AH71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3401,6 +3701,10 @@
         <v>1188.958828493403</v>
       </c>
       <c r="AD72" t="inlineStr"/>
+      <c r="AE72" t="inlineStr"/>
+      <c r="AF72" t="inlineStr"/>
+      <c r="AG72" t="inlineStr"/>
+      <c r="AH72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3439,6 +3743,10 @@
       <c r="AB73" t="inlineStr"/>
       <c r="AC73" t="inlineStr"/>
       <c r="AD73" t="inlineStr"/>
+      <c r="AE73" t="inlineStr"/>
+      <c r="AF73" t="inlineStr"/>
+      <c r="AG73" t="inlineStr"/>
+      <c r="AH73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -3477,6 +3785,10 @@
       <c r="AD74" t="n">
         <v>1113.916530489799</v>
       </c>
+      <c r="AE74" t="inlineStr"/>
+      <c r="AF74" t="inlineStr"/>
+      <c r="AG74" t="inlineStr"/>
+      <c r="AH74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3515,6 +3827,10 @@
       <c r="AB75" t="inlineStr"/>
       <c r="AC75" t="inlineStr"/>
       <c r="AD75" t="inlineStr"/>
+      <c r="AE75" t="inlineStr"/>
+      <c r="AF75" t="inlineStr"/>
+      <c r="AG75" t="inlineStr"/>
+      <c r="AH75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -3553,6 +3869,10 @@
       <c r="AB76" t="inlineStr"/>
       <c r="AC76" t="inlineStr"/>
       <c r="AD76" t="inlineStr"/>
+      <c r="AE76" t="inlineStr"/>
+      <c r="AF76" t="inlineStr"/>
+      <c r="AG76" t="inlineStr"/>
+      <c r="AH76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -3591,6 +3911,10 @@
       <c r="AB77" t="inlineStr"/>
       <c r="AC77" t="inlineStr"/>
       <c r="AD77" t="inlineStr"/>
+      <c r="AE77" t="inlineStr"/>
+      <c r="AF77" t="inlineStr"/>
+      <c r="AG77" t="inlineStr"/>
+      <c r="AH77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -3629,6 +3953,10 @@
       <c r="AB78" t="inlineStr"/>
       <c r="AC78" t="inlineStr"/>
       <c r="AD78" t="inlineStr"/>
+      <c r="AE78" t="inlineStr"/>
+      <c r="AF78" t="inlineStr"/>
+      <c r="AG78" t="inlineStr"/>
+      <c r="AH78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -3667,6 +3995,10 @@
         <v>1139.327236294392</v>
       </c>
       <c r="AD79" t="inlineStr"/>
+      <c r="AE79" t="inlineStr"/>
+      <c r="AF79" t="inlineStr"/>
+      <c r="AG79" t="inlineStr"/>
+      <c r="AH79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -3705,6 +4037,10 @@
       </c>
       <c r="AC80" t="inlineStr"/>
       <c r="AD80" t="inlineStr"/>
+      <c r="AE80" t="inlineStr"/>
+      <c r="AF80" t="inlineStr"/>
+      <c r="AG80" t="inlineStr"/>
+      <c r="AH80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -3743,6 +4079,10 @@
       <c r="AB81" t="inlineStr"/>
       <c r="AC81" t="inlineStr"/>
       <c r="AD81" t="inlineStr"/>
+      <c r="AE81" t="inlineStr"/>
+      <c r="AF81" t="inlineStr"/>
+      <c r="AG81" t="inlineStr"/>
+      <c r="AH81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -3781,6 +4121,10 @@
       <c r="AB82" t="inlineStr"/>
       <c r="AC82" t="inlineStr"/>
       <c r="AD82" t="inlineStr"/>
+      <c r="AE82" t="inlineStr"/>
+      <c r="AF82" t="inlineStr"/>
+      <c r="AG82" t="inlineStr"/>
+      <c r="AH82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -3819,6 +4163,10 @@
       <c r="AB83" t="inlineStr"/>
       <c r="AC83" t="inlineStr"/>
       <c r="AD83" t="inlineStr"/>
+      <c r="AE83" t="inlineStr"/>
+      <c r="AF83" t="inlineStr"/>
+      <c r="AG83" t="inlineStr"/>
+      <c r="AH83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -3857,6 +4205,10 @@
       </c>
       <c r="AC84" t="inlineStr"/>
       <c r="AD84" t="inlineStr"/>
+      <c r="AE84" t="inlineStr"/>
+      <c r="AF84" t="inlineStr"/>
+      <c r="AG84" t="inlineStr"/>
+      <c r="AH84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -3895,6 +4247,10 @@
       <c r="AB85" t="inlineStr"/>
       <c r="AC85" t="inlineStr"/>
       <c r="AD85" t="inlineStr"/>
+      <c r="AE85" t="inlineStr"/>
+      <c r="AF85" t="inlineStr"/>
+      <c r="AG85" t="inlineStr"/>
+      <c r="AH85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3933,6 +4289,10 @@
       <c r="AB86" t="inlineStr"/>
       <c r="AC86" t="inlineStr"/>
       <c r="AD86" t="inlineStr"/>
+      <c r="AE86" t="inlineStr"/>
+      <c r="AF86" t="inlineStr"/>
+      <c r="AG86" t="inlineStr"/>
+      <c r="AH86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3971,6 +4331,10 @@
       <c r="AB87" t="inlineStr"/>
       <c r="AC87" t="inlineStr"/>
       <c r="AD87" t="inlineStr"/>
+      <c r="AE87" t="inlineStr"/>
+      <c r="AF87" t="inlineStr"/>
+      <c r="AG87" t="inlineStr"/>
+      <c r="AH87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -4009,6 +4373,10 @@
       <c r="AB88" t="inlineStr"/>
       <c r="AC88" t="inlineStr"/>
       <c r="AD88" t="inlineStr"/>
+      <c r="AE88" t="inlineStr"/>
+      <c r="AF88" t="inlineStr"/>
+      <c r="AG88" t="inlineStr"/>
+      <c r="AH88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -4047,6 +4415,10 @@
       <c r="AB89" t="inlineStr"/>
       <c r="AC89" t="inlineStr"/>
       <c r="AD89" t="inlineStr"/>
+      <c r="AE89" t="inlineStr"/>
+      <c r="AF89" t="inlineStr"/>
+      <c r="AG89" t="inlineStr"/>
+      <c r="AH89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -4085,6 +4457,10 @@
       <c r="AB90" t="inlineStr"/>
       <c r="AC90" t="inlineStr"/>
       <c r="AD90" t="inlineStr"/>
+      <c r="AE90" t="inlineStr"/>
+      <c r="AF90" t="inlineStr"/>
+      <c r="AG90" t="inlineStr"/>
+      <c r="AH90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -4123,6 +4499,10 @@
       <c r="AB91" t="inlineStr"/>
       <c r="AC91" t="inlineStr"/>
       <c r="AD91" t="inlineStr"/>
+      <c r="AE91" t="inlineStr"/>
+      <c r="AF91" t="inlineStr"/>
+      <c r="AG91" t="inlineStr"/>
+      <c r="AH91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -4161,6 +4541,10 @@
       <c r="AB92" t="inlineStr"/>
       <c r="AC92" t="inlineStr"/>
       <c r="AD92" t="inlineStr"/>
+      <c r="AE92" t="inlineStr"/>
+      <c r="AF92" t="inlineStr"/>
+      <c r="AG92" t="inlineStr"/>
+      <c r="AH92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -4199,6 +4583,10 @@
       <c r="AB93" t="inlineStr"/>
       <c r="AC93" t="inlineStr"/>
       <c r="AD93" t="inlineStr"/>
+      <c r="AE93" t="inlineStr"/>
+      <c r="AF93" t="inlineStr"/>
+      <c r="AG93" t="inlineStr"/>
+      <c r="AH93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -4237,6 +4625,10 @@
       <c r="AB94" t="inlineStr"/>
       <c r="AC94" t="inlineStr"/>
       <c r="AD94" t="inlineStr"/>
+      <c r="AE94" t="inlineStr"/>
+      <c r="AF94" t="inlineStr"/>
+      <c r="AG94" t="inlineStr"/>
+      <c r="AH94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -4275,6 +4667,10 @@
       <c r="AB95" t="inlineStr"/>
       <c r="AC95" t="inlineStr"/>
       <c r="AD95" t="inlineStr"/>
+      <c r="AE95" t="inlineStr"/>
+      <c r="AF95" t="inlineStr"/>
+      <c r="AG95" t="inlineStr"/>
+      <c r="AH95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -4313,6 +4709,10 @@
       <c r="AB96" t="inlineStr"/>
       <c r="AC96" t="inlineStr"/>
       <c r="AD96" t="inlineStr"/>
+      <c r="AE96" t="inlineStr"/>
+      <c r="AF96" t="inlineStr"/>
+      <c r="AG96" t="inlineStr"/>
+      <c r="AH96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -4351,6 +4751,10 @@
       <c r="AB97" t="inlineStr"/>
       <c r="AC97" t="inlineStr"/>
       <c r="AD97" t="inlineStr"/>
+      <c r="AE97" t="inlineStr"/>
+      <c r="AF97" t="inlineStr"/>
+      <c r="AG97" t="inlineStr"/>
+      <c r="AH97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -4389,6 +4793,10 @@
       <c r="AB98" t="inlineStr"/>
       <c r="AC98" t="inlineStr"/>
       <c r="AD98" t="inlineStr"/>
+      <c r="AE98" t="inlineStr"/>
+      <c r="AF98" t="inlineStr"/>
+      <c r="AG98" t="inlineStr"/>
+      <c r="AH98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -4431,6 +4839,10 @@
       <c r="AD99" t="n">
         <v>1058.266119428515</v>
       </c>
+      <c r="AE99" t="inlineStr"/>
+      <c r="AF99" t="inlineStr"/>
+      <c r="AG99" t="inlineStr"/>
+      <c r="AH99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -4473,6 +4885,10 @@
       <c r="AB100" t="inlineStr"/>
       <c r="AC100" t="inlineStr"/>
       <c r="AD100" t="inlineStr"/>
+      <c r="AE100" t="inlineStr"/>
+      <c r="AF100" t="inlineStr"/>
+      <c r="AG100" t="inlineStr"/>
+      <c r="AH100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -4515,6 +4931,10 @@
       <c r="AB101" t="inlineStr"/>
       <c r="AC101" t="inlineStr"/>
       <c r="AD101" t="inlineStr"/>
+      <c r="AE101" t="inlineStr"/>
+      <c r="AF101" t="inlineStr"/>
+      <c r="AG101" t="inlineStr"/>
+      <c r="AH101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -4557,6 +4977,10 @@
       <c r="AB102" t="inlineStr"/>
       <c r="AC102" t="inlineStr"/>
       <c r="AD102" t="inlineStr"/>
+      <c r="AE102" t="inlineStr"/>
+      <c r="AF102" t="inlineStr"/>
+      <c r="AG102" t="inlineStr"/>
+      <c r="AH102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -4599,6 +5023,562 @@
       <c r="AB103" t="inlineStr"/>
       <c r="AC103" t="inlineStr"/>
       <c r="AD103" t="inlineStr"/>
+      <c r="AE103" t="inlineStr"/>
+      <c r="AF103" t="inlineStr"/>
+      <c r="AG103" t="inlineStr"/>
+      <c r="AH103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="n">
+        <v>1544.302477264692</v>
+      </c>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="n">
+        <v>1206.063981098702</v>
+      </c>
+      <c r="I104" t="n">
+        <v>979.4502013604686</v>
+      </c>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr"/>
+      <c r="R104" t="inlineStr"/>
+      <c r="S104" t="inlineStr"/>
+      <c r="T104" t="inlineStr"/>
+      <c r="U104" t="inlineStr"/>
+      <c r="V104" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr"/>
+      <c r="Y104" t="inlineStr"/>
+      <c r="Z104" t="inlineStr"/>
+      <c r="AA104" t="inlineStr"/>
+      <c r="AB104" t="inlineStr"/>
+      <c r="AC104" t="inlineStr"/>
+      <c r="AD104" t="inlineStr"/>
+      <c r="AE104" t="inlineStr"/>
+      <c r="AF104" t="n">
+        <v>1192.819513605344</v>
+      </c>
+      <c r="AG104" t="inlineStr"/>
+      <c r="AH104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="n">
+        <v>1545.742079244441</v>
+      </c>
+      <c r="G105" t="n">
+        <v>1269.209554187589</v>
+      </c>
+      <c r="H105" t="n">
+        <v>1207.503583078451</v>
+      </c>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="n">
+        <v>1137.252855431793</v>
+      </c>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
+      <c r="R105" t="inlineStr"/>
+      <c r="S105" t="inlineStr"/>
+      <c r="T105" t="inlineStr"/>
+      <c r="U105" t="inlineStr"/>
+      <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
+      <c r="Z105" t="inlineStr"/>
+      <c r="AA105" t="inlineStr"/>
+      <c r="AB105" t="inlineStr"/>
+      <c r="AC105" t="inlineStr"/>
+      <c r="AD105" t="inlineStr"/>
+      <c r="AE105" t="inlineStr"/>
+      <c r="AF105" t="inlineStr"/>
+      <c r="AG105" t="inlineStr"/>
+      <c r="AH105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="n">
+        <v>1313.684825654176</v>
+      </c>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="n">
+        <v>1427.419378002535</v>
+      </c>
+      <c r="R106" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
+      <c r="T106" t="n">
+        <v>1162.43448193746</v>
+      </c>
+      <c r="U106" t="inlineStr"/>
+      <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
+      <c r="Z106" t="n">
+        <v>1040.370685155026</v>
+      </c>
+      <c r="AA106" t="inlineStr"/>
+      <c r="AB106" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
+      <c r="AD106" t="inlineStr"/>
+      <c r="AE106" t="inlineStr"/>
+      <c r="AF106" t="inlineStr"/>
+      <c r="AG106" t="inlineStr"/>
+      <c r="AH106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="n">
+        <v>1546.311365205288</v>
+      </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="n">
+        <v>1208.072869039298</v>
+      </c>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
+      <c r="R107" t="n">
+        <v>1183.082625265769</v>
+      </c>
+      <c r="S107" t="inlineStr"/>
+      <c r="T107" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
+      <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
+      <c r="Z107" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
+      <c r="AB107" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
+      <c r="AD107" t="inlineStr"/>
+      <c r="AE107" t="n">
+        <v>1199.430714039153</v>
+      </c>
+      <c r="AF107" t="inlineStr"/>
+      <c r="AG107" t="inlineStr"/>
+      <c r="AH107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="n">
+        <v>1338.099046793333</v>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="n">
+        <v>1521.897144066131</v>
+      </c>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="n">
+        <v>1183.658647900141</v>
+      </c>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="n">
+        <v>1451.833599141692</v>
+      </c>
+      <c r="R108" t="inlineStr"/>
+      <c r="S108" t="inlineStr"/>
+      <c r="T108" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
+      <c r="V108" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
+      <c r="Z108" t="inlineStr"/>
+      <c r="AA108" t="inlineStr"/>
+      <c r="AB108" t="inlineStr"/>
+      <c r="AC108" t="inlineStr"/>
+      <c r="AD108" t="inlineStr"/>
+      <c r="AE108" t="inlineStr"/>
+      <c r="AF108" t="inlineStr"/>
+      <c r="AG108" t="inlineStr"/>
+      <c r="AH108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="n">
+        <v>1498.287424819952</v>
+      </c>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="n">
+        <v>1160.048928653962</v>
+      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="n">
+        <v>1160.862574677972</v>
+      </c>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
+      <c r="T109" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
+      <c r="Z109" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
+      <c r="AB109" t="inlineStr"/>
+      <c r="AC109" t="inlineStr"/>
+      <c r="AD109" t="inlineStr"/>
+      <c r="AE109" t="inlineStr"/>
+      <c r="AF109" t="n">
+        <v>1216.429232851523</v>
+      </c>
+      <c r="AG109" t="inlineStr"/>
+      <c r="AH109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="n">
+        <v>1303.641964193648</v>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="n">
+        <v>1303.666636787274</v>
+      </c>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="n">
+        <v>1417.376516542007</v>
+      </c>
+      <c r="R110" t="n">
+        <v>1217.539707865454</v>
+      </c>
+      <c r="S110" t="inlineStr"/>
+      <c r="T110" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
+      <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
+      <c r="Z110" t="inlineStr"/>
+      <c r="AA110" t="inlineStr"/>
+      <c r="AB110" t="inlineStr"/>
+      <c r="AC110" t="inlineStr"/>
+      <c r="AD110" t="inlineStr"/>
+      <c r="AE110" t="inlineStr"/>
+      <c r="AF110" t="inlineStr"/>
+      <c r="AG110" t="inlineStr"/>
+      <c r="AH110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="n">
+        <v>1275.183515985441</v>
+      </c>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="n">
+        <v>1189.345695479805</v>
+      </c>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
+      <c r="R111" t="n">
+        <v>1189.056587063621</v>
+      </c>
+      <c r="S111" t="inlineStr"/>
+      <c r="T111" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
+      <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
+      <c r="Z111" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
+      <c r="AB111" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
+      <c r="AD111" t="inlineStr"/>
+      <c r="AE111" t="inlineStr"/>
+      <c r="AF111" t="n">
+        <v>1244.912353653355</v>
+      </c>
+      <c r="AG111" t="inlineStr"/>
+      <c r="AH111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="n">
+        <v>1504.772979793352</v>
+      </c>
+      <c r="G112" t="n">
+        <v>1281.669070958841</v>
+      </c>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
+      <c r="R112" t="inlineStr"/>
+      <c r="S112" t="n">
+        <v>1389.845978659066</v>
+      </c>
+      <c r="T112" t="inlineStr"/>
+      <c r="U112" t="inlineStr"/>
+      <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
+      <c r="Z112" t="inlineStr"/>
+      <c r="AA112" t="inlineStr"/>
+      <c r="AB112" t="inlineStr"/>
+      <c r="AC112" t="inlineStr"/>
+      <c r="AD112" t="inlineStr"/>
+      <c r="AE112" t="inlineStr"/>
+      <c r="AF112" t="inlineStr"/>
+      <c r="AG112" t="n">
+        <v>1193.5144450266</v>
+      </c>
+      <c r="AH112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="n">
+        <v>1536.548325813933</v>
+      </c>
+      <c r="G113" t="n">
+        <v>1313.444416979422</v>
+      </c>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="n">
+        <v>1201.692490161548</v>
+      </c>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="n">
+        <v>1385.601170521426</v>
+      </c>
+      <c r="R113" t="inlineStr"/>
+      <c r="S113" t="inlineStr"/>
+      <c r="T113" t="inlineStr"/>
+      <c r="U113" t="inlineStr"/>
+      <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
+      <c r="Z113" t="inlineStr"/>
+      <c r="AA113" t="inlineStr"/>
+      <c r="AB113" t="inlineStr"/>
+      <c r="AC113" t="inlineStr"/>
+      <c r="AD113" t="inlineStr"/>
+      <c r="AE113" t="inlineStr"/>
+      <c r="AF113" t="inlineStr"/>
+      <c r="AG113" t="inlineStr"/>
+      <c r="AH113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="n">
+        <v>1558.36774250098</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1335.263833666469</v>
+      </c>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="n">
+        <v>1167.526278792758</v>
+      </c>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
+      <c r="R114" t="inlineStr"/>
+      <c r="S114" t="inlineStr"/>
+      <c r="T114" t="inlineStr"/>
+      <c r="U114" t="inlineStr"/>
+      <c r="V114" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
+      <c r="Z114" t="inlineStr"/>
+      <c r="AA114" t="inlineStr"/>
+      <c r="AB114" t="inlineStr"/>
+      <c r="AC114" t="inlineStr"/>
+      <c r="AD114" t="inlineStr"/>
+      <c r="AE114" t="inlineStr"/>
+      <c r="AF114" t="inlineStr"/>
+      <c r="AG114" t="inlineStr"/>
+      <c r="AH114" t="n">
+        <v>1178.180583312953</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="n">
+        <v>1578.068408583175</v>
+      </c>
+      <c r="G115" t="n">
+        <v>1354.964499748664</v>
+      </c>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
+      <c r="R115" t="inlineStr"/>
+      <c r="S115" t="inlineStr"/>
+      <c r="T115" t="n">
+        <v>1142.733815855265</v>
+      </c>
+      <c r="U115" t="inlineStr"/>
+      <c r="V115" t="inlineStr"/>
+      <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
+      <c r="Z115" t="inlineStr"/>
+      <c r="AA115" t="inlineStr"/>
+      <c r="AB115" t="inlineStr"/>
+      <c r="AC115" t="inlineStr"/>
+      <c r="AD115" t="inlineStr"/>
+      <c r="AE115" t="n">
+        <v>1179.730047956958</v>
+      </c>
+      <c r="AF115" t="inlineStr"/>
+      <c r="AG115" t="inlineStr"/>
+      <c r="AH115" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>